<commit_message>
Added the rest of the new NORTH things
</commit_message>
<xml_diff>
--- a/figures/Diagram_identification.xlsx
+++ b/figures/Diagram_identification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/coadw_lunet_lboro_ac_uk/Documents/Dokumente/Universität/Loughborough/Master_thesis/Programming/data_curation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/coadw_lunet_lboro_ac_uk/Documents/Dokumente/Universität/Loughborough/Master_thesis/Programming/data_curation/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{FFF08D63-2973-4B04-B4CF-C93C1A66318B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{295A258E-0C68-450D-9A62-C99CC2916556}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="8_{FFF08D63-2973-4B04-B4CF-C93C1A66318B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{538D4E2F-E66D-4572-BF04-B0C8B93B80F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8D00E84D-9986-4B19-A1AB-6B1D6F0EE8B1}"/>
   </bookViews>
@@ -174,6 +174,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF196B24"/>
+      <color rgb="FF0B3041"/>
+      <color rgb="FF215F9A"/>
       <color rgb="FF306AEC"/>
     </mruColors>
   </colors>
@@ -362,34 +365,115 @@
               <c:idx val="0"/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="72000" tIns="36000" rIns="72000" bIns="36000" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:fld id="{F34560F8-6228-4B43-B60B-72F9439DF666}" type="CATEGORYNAME">
                       <a:rPr lang="en-US" b="1"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[RUBRIKENNAME]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" b="1" baseline="0"/>
                   </a:p>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:fld id="{E6473CC1-B063-4D50-A679-EADA6EED2945}" type="VALUE">
                       <a:rPr lang="en-US"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>(</a:t>
+                    </a:r>
                     <a:fld id="{8C4058AF-56B9-4764-BD8E-503A59EABAA8}" type="PERCENTAGE">
                       <a:rPr lang="en-US"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-DE"/>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="72000" tIns="36000" rIns="72000" bIns="36000" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -401,6 +485,21 @@
 </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.13386451995267831"/>
+                      <c:h val="0.11829145390634332"/>
+                    </c:manualLayout>
+                  </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -413,8 +512,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10928961748633879"/>
-                  <c:y val="-7.8499108376480262E-2"/>
+                  <c:x val="-1.8594452257543536E-2"/>
+                  <c:y val="-7.810983427220311E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -425,7 +524,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -435,7 +534,7 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -443,7 +542,7 @@
                       <a:t>Found in </a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -451,7 +550,7 @@
                       <a:t>Compounds</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -459,29 +558,29 @@
                       <a:t> after </a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>LLM name extraction</a:t>
+                      <a:t>LLM name extraction:</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>; </a:t>
+                      <a:t> </a:t>
                     </a:r>
                     <a:fld id="{EA77BC39-BF2E-4F0B-8F2F-939ED3CA425A}" type="VALUE">
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -490,21 +589,21 @@
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>; </a:t>
+                      <a:t> (</a:t>
                     </a:r>
                     <a:fld id="{107459AB-3647-477F-BD64-B6EDD8F96E58}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -512,11 +611,14 @@
                       </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" sz="1000" baseline="0">
-                      <a:solidFill>
-                        <a:sysClr val="windowText" lastClr="000000"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -530,10 +632,7 @@
                 </a:solidFill>
                 <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:sysClr>
+                    <a:schemeClr val="accent6"/>
                   </a:solidFill>
                   <a:prstDash val="solid"/>
                   <a:round/>
@@ -564,7 +663,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
@@ -600,8 +699,8 @@
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.23996170560647131"/>
-                      <c:h val="7.5292992747491252E-2"/>
+                      <c:w val="0.2648767264747644"/>
+                      <c:h val="7.6071501991212848E-2"/>
                     </c:manualLayout>
                   </c15:layout>
                   <c15:dlblFieldTable/>
@@ -616,8 +715,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.4368163747925273E-2"/>
-                  <c:y val="-1.1446745321394004E-4"/>
+                  <c:x val="-1.834992034130881E-2"/>
+                  <c:y val="-5.2486132546075335E-4"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -628,7 +727,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -638,7 +737,7 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -646,7 +745,7 @@
                       <a:t>Found in </a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -654,7 +753,7 @@
                       <a:t>Substances</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -662,29 +761,29 @@
                       <a:t> after </a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" b="1" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>LLM name extraction</a:t>
+                      <a:t>LLM name extraction:</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>; </a:t>
+                      <a:t> </a:t>
                     </a:r>
                     <a:fld id="{42367EB0-57E6-4A1B-81A7-E12308BF7351}" type="VALUE">
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -693,21 +792,21 @@
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>; </a:t>
+                      <a:t> (</a:t>
                     </a:r>
                     <a:fld id="{DF01BD90-1379-4D54-AA02-25103D64C867}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -715,11 +814,14 @@
                       </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0">
-                      <a:solidFill>
-                        <a:sysClr val="windowText" lastClr="000000"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -729,10 +831,7 @@
                 </a:solidFill>
                 <a:ln>
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:sysClr>
+                    <a:srgbClr val="196B24"/>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -744,7 +843,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
@@ -768,8 +867,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.24552832065965474"/>
-                      <c:h val="7.6892281568325588E-2"/>
+                      <c:w val="0.26480430586801151"/>
+                      <c:h val="7.6071571823089795E-2"/>
                     </c:manualLayout>
                   </c15:layout>
                   <c15:dlblFieldTable/>
@@ -784,15 +883,27 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.4678268530296377E-2"/>
-                  <c:y val="-4.9156197106287377E-3"/>
+                  <c:x val="-1.7439869196678285E-2"/>
+                  <c:y val="-2.488035990036809E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>Found </a:t>
@@ -803,11 +914,11 @@
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> in PubChem's </a:t>
+                      <a:t> in </a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" b="1" baseline="0"/>
-                      <a:t>Compounds</a:t>
+                      <a:t>Compounds:</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
@@ -815,22 +926,67 @@
                     </a:r>
                     <a:fld id="{434D3142-FF6A-4CAF-860A-28C952333E71}" type="VALUE">
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
+                      <a:t> (</a:t>
                     </a:r>
                     <a:fld id="{C84FFC41-8F82-460D-B754-B58AE9B8CCC3}" type="PERCENTAGE">
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="215F9A"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -841,6 +997,12 @@
               <c:separator>; </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.20628215100712963"/>
+                      <c:h val="8.9902766700015208E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -853,15 +1015,27 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.4540302019415106E-2"/>
-                  <c:y val="-9.0118653636482429E-17"/>
+                  <c:x val="-1.6885544568331537E-2"/>
+                  <c:y val="8.9873597023784474E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>Found </a:t>
@@ -872,11 +1046,11 @@
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t> in PubChem's </a:t>
+                      <a:t> in </a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" b="1" baseline="0"/>
-                      <a:t>Substances</a:t>
+                      <a:t>Substances:</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
@@ -884,22 +1058,67 @@
                     </a:r>
                     <a:fld id="{4A0D9799-E0BF-4FD8-AE14-8F164B25C66B}" type="VALUE">
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>; </a:t>
+                      <a:t> (</a:t>
                     </a:r>
                     <a:fld id="{8D95F517-3E64-481F-A95A-79CA6390EF75}" type="PERCENTAGE">
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:pPr/>
+                      <a:pPr>
+                        <a:defRPr sz="1100">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                        </a:defRPr>
+                      </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="0B3041"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -910,6 +1129,12 @@
               <c:separator>; </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.20628215100712963"/>
+                      <c:h val="8.9902766700015208E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -922,19 +1147,19 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15059090974283959"/>
-                  <c:y val="9.5616463242641124E-8"/>
+                  <c:x val="-0.15944600834306966"/>
+                  <c:y val="-1.3934389129085399E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="72000" tIns="36000" rIns="72000" bIns="36000" anchor="ctr" anchorCtr="1">
                     <a:noAutofit/>
                   </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -944,7 +1169,7 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" b="1" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -952,7 +1177,7 @@
                       <a:t>Identified</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -960,13 +1185,13 @@
                       <a:t> </a:t>
                     </a:r>
                     <a:fld id="{EE887BFB-006A-4957-A8A7-B8171D8353B4}" type="VALUE">
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -975,20 +1200,28 @@
                       <a:t>[WERT]</a:t>
                     </a:fld>
                     <a:br>
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                     </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>(</a:t>
+                    </a:r>
                     <a:fld id="{3310328D-CA3B-4D74-A6EB-B8BC9577C709}" type="PERCENTAGE">
-                      <a:rPr lang="en-US" sz="1000" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:pPr>
-                        <a:defRPr sz="1000">
+                        <a:defRPr sz="1100">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
@@ -996,11 +1229,14 @@
                       </a:pPr>
                       <a:t>[PROZENTSATZ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" sz="1000" baseline="0">
-                      <a:solidFill>
-                        <a:sysClr val="windowText" lastClr="000000"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>)</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1010,22 +1246,19 @@
                 </a:solidFill>
                 <a:ln>
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:sysClr>
+                    <a:schemeClr val="bg1"/>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
               <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="72000" tIns="36000" rIns="72000" bIns="36000" anchor="ctr" anchorCtr="1">
                   <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
@@ -1050,8 +1283,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="9.4052895027465833E-2"/>
-                      <c:h val="9.9538650564854239E-2"/>
+                      <c:w val="0.12356724918708767"/>
+                      <c:h val="0.11638932915244606"/>
                     </c:manualLayout>
                   </c15:layout>
                   <c15:dlblFieldTable/>
@@ -1083,7 +1316,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1138,19 +1371,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1734</c:v>
+                  <c:v>1666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>227</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>437</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1315,8 +1548,8 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7C2DBFA6-0B74-4153-82F0-A8EDDA96BB3A}" type="CELLRANGE">
-                      <a:rPr lang="en-US" sz="1050">
+                    <a:fld id="{C0529798-EE6A-45AE-BA6F-C0FECF88689B}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -1338,7 +1571,7 @@
                       </a:rPr>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{412551D2-67FB-48E4-B65F-DE0B4C7B58EA}" type="CATEGORYNAME">
+                    <a:fld id="{E1F9C822-4769-40DB-96F4-01020E6E6ED2}" type="CATEGORYNAME">
                       <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
@@ -1473,8 +1706,8 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{8FAE6B0B-33C9-461F-A1DF-1F0A730093BF}" type="CELLRANGE">
-                      <a:rPr lang="en-US" sz="1050">
+                    <a:fld id="{80D6018D-3783-4361-8126-D6439D277FDA}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -1496,7 +1729,7 @@
                       </a:rPr>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{72CBE0B7-8F78-43DE-8A56-15DB9F201CC4}" type="CATEGORYNAME">
+                    <a:fld id="{B3A4010C-FF04-4D40-B77C-D558F1F84993}" type="CATEGORYNAME">
                       <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
@@ -1631,8 +1864,8 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{DA7ABE03-E6B9-4F7C-9BDB-B300E62E1C14}" type="CELLRANGE">
-                      <a:rPr lang="en-US" sz="1050">
+                    <a:fld id="{5438F0B6-7A9A-4C43-A2EF-965E0E21A723}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
                         </a:solidFill>
@@ -1654,7 +1887,7 @@
                       </a:rPr>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{183FBA73-178D-44A9-A9FF-3263CFAC678F}" type="CATEGORYNAME">
+                    <a:fld id="{B08896E2-CD62-48CA-A549-4EE40A316C13}" type="CATEGORYNAME">
                       <a:rPr lang="en-US" sz="1050" baseline="0">
                         <a:solidFill>
                           <a:sysClr val="windowText" lastClr="000000"/>
@@ -1845,13 +2078,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>41083</c:v>
+                  <c:v>40950</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39396</c:v>
+                  <c:v>39643</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37664</c:v>
+                  <c:v>37713</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,13 +2096,13 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>95,28%</c:v>
+                    <c:v>94,97%</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>91,37%</c:v>
+                    <c:v>91,94%</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>87,35%</c:v>
+                    <c:v>87,46%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1929,13 +2162,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2036</c:v>
+                  <c:v>2169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3723</c:v>
+                  <c:v>3476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5455</c:v>
+                  <c:v>5406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2155,13 +2388,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>37664</c:v>
+                  <c:v>37713</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39396</c:v>
+                  <c:v>39642</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41083</c:v>
+                  <c:v>40950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2225,13 +2458,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5455</c:v>
+                  <c:v>5406</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3723</c:v>
+                  <c:v>3477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2036</c:v>
+                  <c:v>2169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,15 +2513,57 @@
           <c:orientation val="minMax"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="947590304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4089,10 +4364,10 @@
       <xdr:rowOff>87586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405085</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>163786</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>284656</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>65690</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4107,8 +4382,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5003361" y="273707"/>
-          <a:ext cx="4598276" cy="2681889"/>
+          <a:off x="4977085" y="278086"/>
+          <a:ext cx="5975571" cy="3407104"/>
           <a:chOff x="4598276" y="3722414"/>
           <a:chExt cx="4598276" cy="2681889"/>
         </a:xfrm>
@@ -4149,7 +4424,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4732061" y="4148968"/>
+            <a:off x="4740436" y="4104858"/>
             <a:ext cx="3722892" cy="231022"/>
           </a:xfrm>
           <a:prstGeom prst="rightArrow">
@@ -4189,40 +4464,26 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1100">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>For</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1100">
-                <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>For </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>95.28</a:t>
+              <a:t>94.97</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> %</a:t>
+              <a:t>%</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1100" baseline="0">
@@ -4230,24 +4491,12 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>of cells, the </a:t>
+              <a:t> of cells, the </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>ETL</a:t>
@@ -4258,23 +4507,11 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>was identified.</a:t>
+              <a:t> was identified.</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:endParaRPr>
           </a:p>
@@ -4293,7 +4530,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4720947" y="5748168"/>
+            <a:off x="4729323" y="5651126"/>
             <a:ext cx="3179914" cy="228043"/>
           </a:xfrm>
           <a:prstGeom prst="rightArrow">
@@ -4333,9 +4570,7 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1100">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>For </a:t>
@@ -4343,29 +4578,23 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>87.35</a:t>
+              <a:t>87.46</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> %</a:t>
+              <a:t>%</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t> of cells, </a:t>
@@ -4373,28 +4602,30 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>both CTLs </a:t>
+              <a:t>both CTLs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>were identified.</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:endParaRPr>
           </a:p>
@@ -4413,7 +4644,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4728127" y="4959268"/>
+            <a:off x="4753254" y="4879871"/>
             <a:ext cx="3467914" cy="231022"/>
           </a:xfrm>
           <a:prstGeom prst="rightArrow">
@@ -4453,9 +4684,7 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1100">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>For </a:t>
@@ -4463,29 +4692,23 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>91.37</a:t>
+              <a:t>91.94</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> %</a:t>
+              <a:t>%</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" sz="1100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t> of cells, the </a:t>
@@ -4493,9 +4716,7 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="196B24"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>HTL</a:t>
@@ -4503,18 +4724,14 @@
             <a:r>
               <a:rPr lang="de-DE" sz="1100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
               <a:t> was identified.</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:endParaRPr>
           </a:p>
@@ -4845,19 +5062,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFF586-6CB0-4BA2-91A5-7B1CF9837E78}">
   <dimension ref="B12:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12">
-        <f>2559-825</f>
-        <v>1734</v>
+        <f>2534-868</f>
+        <v>1666</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -4865,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -4873,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -4881,7 +5101,7 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -4889,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>437</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -4902,8 +5122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A376227E-6BBC-46B4-AB1B-0A06CB989B62}">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4924,16 +5144,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <f>40802+C5</f>
-        <v>41083</v>
+        <v>40950</v>
       </c>
       <c r="D3" s="1">
-        <f>36770+D5</f>
-        <v>39396</v>
+        <v>39643</v>
       </c>
       <c r="E3" s="1">
-        <f>37633+E5</f>
-        <v>37664</v>
+        <v>37713</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -4942,15 +5159,15 @@
       </c>
       <c r="C4">
         <f>E6-C3</f>
-        <v>2036</v>
+        <v>2169</v>
       </c>
       <c r="D4">
         <f>E6-D3</f>
-        <v>3723</v>
+        <v>3476</v>
       </c>
       <c r="E4">
         <f>E6-E3</f>
-        <v>5455</v>
+        <v>5406</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -4982,15 +5199,15 @@
       </c>
       <c r="C9" s="3">
         <f>C3/$E$6</f>
-        <v>0.95278183631345814</v>
+        <v>0.94969734919640991</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ref="D9:E9" si="0">D3/$E$6</f>
-        <v>0.91365755235511026</v>
+        <v>0.91938588557248546</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.87348964493610703</v>
+        <v>0.87462603492659852</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -5009,13 +5226,13 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>37664</v>
+        <v>37713</v>
       </c>
       <c r="D14">
-        <v>39396</v>
+        <v>39642</v>
       </c>
       <c r="E14">
-        <v>41083</v>
+        <v>40950</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -5023,13 +5240,16 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>5455</v>
+        <f>$E$17-C14</f>
+        <v>5406</v>
       </c>
       <c r="D15">
-        <v>3723</v>
+        <f t="shared" ref="D15:E15" si="1">$E$17-D14</f>
+        <v>3477</v>
       </c>
       <c r="E15">
-        <v>2036</v>
+        <f t="shared" si="1"/>
+        <v>2169</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -5056,13 +5276,16 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="3">
-        <v>0.87348964493610703</v>
+        <f>C14/$E$17</f>
+        <v>0.87462603492659852</v>
       </c>
       <c r="D19" s="3">
-        <v>0.91365755235511026</v>
+        <f t="shared" ref="D19:E19" si="2">D14/$E$17</f>
+        <v>0.91936269394002645</v>
       </c>
       <c r="E19" s="3">
-        <v>0.95278183631345814</v>
+        <f t="shared" si="2"/>
+        <v>0.94969734919640991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>